<commit_message>
STAGE-6: Added results and formatted files
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cezar\Desktop\Disertatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CE887F-46FB-4A31-A338-6E3968E0FD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2A04A5-3B0A-4443-A246-C2EFFCC5A967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="38">
   <si>
     <t>Model</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t>end_to_end_v7</t>
+  </si>
+  <si>
+    <t>End to End V10</t>
+  </si>
+  <si>
+    <t>end_to_end_v10</t>
   </si>
 </sst>
 </file>
@@ -156,7 +162,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,6 +205,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -329,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -373,6 +385,9 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="G7" sqref="C7:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,6 +1522,35 @@
       </c>
       <c r="I30" s="42" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="44">
+        <v>1</v>
+      </c>
+      <c r="C31" s="44">
+        <v>64</v>
+      </c>
+      <c r="D31" s="44">
+        <v>0.87939999999999996</v>
+      </c>
+      <c r="E31" s="44">
+        <v>0.98040000000000005</v>
+      </c>
+      <c r="F31" s="44">
+        <v>33.946899999999999</v>
+      </c>
+      <c r="G31" s="44">
+        <v>0.74150000000000005</v>
+      </c>
+      <c r="H31" s="44">
+        <v>30</v>
+      </c>
+      <c r="I31" s="45" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>